<commit_message>
Updated the scripts for reading all riskperception datasets
</commit_message>
<xml_diff>
--- a/Datasets/housinggame_session_20_251007_surveys/251009_251007_WhereWeMove sessions - presurvey.xlsx
+++ b/Datasets/housinggame_session_20_251007_surveys/251009_251007_WhereWeMove sessions - presurvey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/jcortesarevalo_tudelft_nl/Documents/Documents/TUDelft/18_Game Data Analysis/R data analysis BEPs/Datasets/housinggame_session_20_251007_surveys/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F267ED7BEE40FE1B69EAED488EA404700F25161E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C8D3BA4-1F6E-434F-93BC-B0ABC52D9E03}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_F267ED7BEE40FE1B69EAED488EA404700F25161E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5719907-76E2-4A4A-A450-52F6EB3B80E5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -251,9 +251,6 @@
     <t/>
   </si>
   <si>
-    <t>Nee, ik heb geen ervaring met overstromingen.</t>
-  </si>
-  <si>
     <t>Nooit</t>
   </si>
   <si>
@@ -299,9 +296,6 @@
     <t>Eén keer per dag</t>
   </si>
   <si>
-    <t>Neutraal,</t>
-  </si>
-  <si>
     <t>Een kleine toename</t>
   </si>
   <si>
@@ -353,9 +347,6 @@
     <t>Productmanagement</t>
   </si>
   <si>
-    <t>Ja, met enige verstoringen of schade.</t>
-  </si>
-  <si>
     <t>R_2VsYdsHWvlxuHOv</t>
   </si>
   <si>
@@ -374,9 +365,6 @@
     <t>t2p4</t>
   </si>
   <si>
-    <t>Ja, met lichte verstoringen of schade.</t>
-  </si>
-  <si>
     <t>Waarschijnlijk</t>
   </si>
   <si>
@@ -407,9 +395,6 @@
     <t>T2p6</t>
   </si>
   <si>
-    <t>Ja, maar zonder verstoringen of schade.</t>
-  </si>
-  <si>
     <t>Ik zou lichte schade kunnen oplopen</t>
   </si>
   <si>
@@ -494,9 +479,6 @@
     <t>Taxateur/Schade-expert</t>
   </si>
   <si>
-    <t>Ja, met ernstige verstoringen of schade.</t>
-  </si>
-  <si>
     <t>R_2CNdiea5wAsJvBz</t>
   </si>
   <si>
@@ -528,6 +510,24 @@
   </si>
   <si>
     <t>t2p2</t>
+  </si>
+  <si>
+    <t>Nee, ik heb geen ervaring met overstromingen</t>
+  </si>
+  <si>
+    <t>Ja, met enige verstoringen of schade</t>
+  </si>
+  <si>
+    <t>Ja, met lichte verstoringen of schade</t>
+  </si>
+  <si>
+    <t>Ja, maar zonder verstoringen of schade</t>
+  </si>
+  <si>
+    <t>Ja, met ernstige verstoringen of schade</t>
+  </si>
+  <si>
+    <t>Neutraal</t>
   </si>
 </sst>
 </file>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection sqref="A1:AH1"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1252,7 +1252,7 @@
         <v>45937.248254502316</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>66</v>
@@ -1264,76 +1264,76 @@
         <v>70</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>70</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="U4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="W4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="W4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="Y4" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AB4" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="AC4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH4" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -1356,7 +1356,7 @@
         <v>45937.250662881946</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>66</v>
@@ -1368,7 +1368,7 @@
         <v>68</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>69</v>
@@ -1377,67 +1377,67 @@
         <v>70</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="X5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="U5" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="V5" s="2" t="s">
+      <c r="Y5" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="W5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="X5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Y5" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="AC5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:34" ht="174" x14ac:dyDescent="0.35">
@@ -1460,7 +1460,7 @@
         <v>45937.250705486113</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>66</v>
@@ -1472,76 +1472,76 @@
         <v>68</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>70</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="R6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="T6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="Q6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="U6" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="X6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="W6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="Y6" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="188.5" x14ac:dyDescent="0.35">
@@ -1564,7 +1564,7 @@
         <v>45937.250719328702</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>66</v>
@@ -1576,76 +1576,76 @@
         <v>68</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="N7" s="2" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
       <c r="O7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="X7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="X7" s="2" t="s">
+      <c r="Y7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD7" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Y7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD7" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="AE7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -1668,7 +1668,7 @@
         <v>45937.250817812499</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>66</v>
@@ -1680,76 +1680,76 @@
         <v>68</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="Q8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="T8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="W8" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AA8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AB8" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="AC8" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF8" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH8" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="AH8" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -1772,7 +1772,7 @@
         <v>45937.250835729166</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>66</v>
@@ -1784,76 +1784,76 @@
         <v>68</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>70</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AF9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -1876,7 +1876,7 @@
         <v>45937.251459236111</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>66</v>
@@ -1888,76 +1888,76 @@
         <v>68</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
       <c r="O10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="X10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="X10" s="2" t="s">
+      <c r="Y10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD10" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Y10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD10" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="AE10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="174" x14ac:dyDescent="0.35">
@@ -1980,7 +1980,7 @@
         <v>45937.251572372683</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>66</v>
@@ -1992,76 +1992,76 @@
         <v>68</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>70</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -2084,7 +2084,7 @@
         <v>45937.251981296293</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>66</v>
@@ -2096,76 +2096,76 @@
         <v>68</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>70</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>123</v>
+        <v>161</v>
       </c>
       <c r="O12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="V12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="W12" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -2188,7 +2188,7 @@
         <v>45937.252174247682</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>66</v>
@@ -2200,76 +2200,76 @@
         <v>68</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AC13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH13" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="AG13" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH13" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -2292,7 +2292,7 @@
         <v>45937.252205034725</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>66</v>
@@ -2304,76 +2304,76 @@
         <v>68</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="V14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="R14" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="V14" s="2" t="s">
+      <c r="W14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="W14" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="X14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB14" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Y14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA14" s="2" t="s">
+      <c r="AC14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AB14" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG14" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="AH14" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -2396,7 +2396,7 @@
         <v>45937.252322499997</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>66</v>
@@ -2408,76 +2408,76 @@
         <v>68</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="V15" s="2" t="s">
+      <c r="W15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="W15" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="X15" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AA15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH15" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="AB15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG15" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH15" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -2500,7 +2500,7 @@
         <v>45937.252370150462</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>66</v>
@@ -2512,76 +2512,76 @@
         <v>68</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
       <c r="O16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="T16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="Q16" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="T16" s="2" t="s">
+      <c r="X16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="U16" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="W16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="X16" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="Y16" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AB16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF16" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="AG16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -2604,7 +2604,7 @@
         <v>45937.252417337964</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>66</v>
@@ -2616,76 +2616,76 @@
         <v>68</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
       <c r="O17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="V17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="P17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="V17" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="W17" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AC17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AE17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AG17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH17" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -2708,7 +2708,7 @@
         <v>45937.252912488424</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>66</v>
@@ -2720,76 +2720,76 @@
         <v>68</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="W18" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y18" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="Z18" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB18" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AC18" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE18" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AF18" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG18" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AH18" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -2812,7 +2812,7 @@
         <v>45937.252994618058</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>66</v>
@@ -2824,7 +2824,7 @@
         <v>68</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>69</v>
@@ -2833,67 +2833,67 @@
         <v>70</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="X19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P19" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R19" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="S19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="T19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="V19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="W19" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="X19" s="2" t="s">
+      <c r="Y19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB19" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Y19" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB19" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="AC19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -2916,7 +2916,7 @@
         <v>45937.253339201387</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>66</v>
@@ -2928,76 +2928,76 @@
         <v>68</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="V20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="X20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="S20" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="T20" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U20" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="V20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="W20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="X20" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="Y20" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z20" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AA20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AB20" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="AC20" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AD20" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AE20" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF20" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG20" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AH20" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -3020,7 +3020,7 @@
         <v>45937.253520937498</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>66</v>
@@ -3032,76 +3032,76 @@
         <v>68</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="O21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="X21" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="V21" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="W21" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="X21" s="2" t="s">
+      <c r="Y21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Y21" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD21" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="AE21" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF21" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AG21" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH21" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -3124,7 +3124,7 @@
         <v>45937.25383548611</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>66</v>
@@ -3136,76 +3136,76 @@
         <v>68</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>70</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="O22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="P22" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="Q22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="U22" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="R22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="V22" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="X22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="W22" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="X22" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="Y22" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB22" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AC22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AG22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AH22" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:34" ht="188.5" x14ac:dyDescent="0.35">
@@ -3228,7 +3228,7 @@
         <v>45937.254022986112</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>66</v>
@@ -3240,76 +3240,76 @@
         <v>68</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>70</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="P23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P23" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="Q23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="R23" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="S23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="U23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="U23" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="V23" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="X23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Y23" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="Z23" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AA23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH23" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:34" ht="188.5" x14ac:dyDescent="0.35">
@@ -3332,7 +3332,7 @@
         <v>45937.254370590279</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>66</v>
@@ -3344,76 +3344,76 @@
         <v>68</v>
       </c>
       <c r="K24" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N24" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="L24" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="O24" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Z24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AC24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD24" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AE24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH24" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -3436,7 +3436,7 @@
         <v>45937.254578773151</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>66</v>
@@ -3448,76 +3448,76 @@
         <v>68</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P25" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="P25" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="Q25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U25" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="R25" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="S25" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="T25" s="2" t="s">
+      <c r="V25" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U25" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="V25" s="2" t="s">
+      <c r="W25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="W25" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="X25" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Y25" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB25" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC25" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AD25" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE25" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF25" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG25" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:34" ht="232" x14ac:dyDescent="0.35">
@@ -3540,7 +3540,7 @@
         <v>45937.256146608794</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>66</v>
@@ -3552,7 +3552,7 @@
         <v>68</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>69</v>
@@ -3561,74 +3561,74 @@
         <v>70</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="U26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V26" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="T26" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U26" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="V26" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="W26" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Z26" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA26" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB26" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AC26" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AD26" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE26" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF26" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG26" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AH26" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:AH27" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E2:E3 G2:G3 H2:H3 I2:I3 J2:J3 K2:K3 L2:L3 M2:M3 N2:N3 O2:O3 P2:P3 Q2:Q3 R2:R3 S2:S3 T2:T3 U2:U3 V2:V3 W2:W3 X2:X3 Y2:Y3 Z2:Z3 AA2:AA3 AB2:AB3 AC2:AC3 AD2:AD3 AE2:AE3 AF2:AF3 AG2:AG3 AH2:AH3 E4:E26 G4:G26 H4:H26 I4:I26 J4:J26 K4:K26 L4:L26 M4:M26 N4:N26 O4:O26 P4:P26 Q4:Q26 R4:R26 S4:S26 T4:T26 U4:U26 V4:V26 W4:W26 X4:X26 Y4:Y26 Z4:Z26 AA4:AA26 AB4:AB26 AC4:AC26 AD4:AD26 AE4:AE26 AF4:AF26 AG4:AG26 AH4:AH26" numberStoredAsText="1"/>
+    <ignoredError sqref="E2:E3 G2:G3 H2:H3 I2:I3 J2:J3 K2:K3 L2:L3 M2:M3 N2:N3 O2:O3 P2:P3 Q2:Q3 R2:R3 S2:S3 T2:T3 U2:U3 V2:V3 W2:W3 X2:X3 Y2:Y3 Z2:Z3 AA2:AA3 AB2:AB3 AC2:AC3 AD2:AD3 AE2:AE3 AF2:AF3 AG2:AG3 AH2:AH3 E4:E26 G4:G26 H4:H26 I4:I26 J4:J26 K4:K26 L4:L26 M4:M26 O4:O26 P4:P26 Q4:Q26 R4:R26 S4:S26 T4:T26 U4:U26 V5 W4:W26 X4:X26 Y4:Y26 Z4:Z26 AA4:AA26 AB4:AB26 AC4:AC26 AD4:AD26 AE4:AE26 AF4:AF26 AG4:AG26 AH4:AH26 V7:V21 V23:V26" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>